<commit_message>
fix: mail in dossier, signature in deal
</commit_message>
<xml_diff>
--- a/methods.xlsx
+++ b/methods.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20384"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AF8070-5DE2-4066-867F-B9DBC4832079}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42252187-3D2F-434A-8E9F-666992F34CF2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="49">
   <si>
     <t>http://localhost:8083/statement</t>
   </si>
@@ -144,6 +144,30 @@
   </si>
   <si>
     <t>http://localhost:8085/statement/select</t>
+  </si>
+  <si>
+    <t>http://localhost:8085/registration/{statementId}</t>
+  </si>
+  <si>
+    <t>http://localhost:8085/deny/{statementId}</t>
+  </si>
+  <si>
+    <t>http://localhost:8085/admin/statement/{statementId}/status</t>
+  </si>
+  <si>
+    <t>http://localhost:8085/admin/statement/{statementId}</t>
+  </si>
+  <si>
+    <t>http://localhost:8085/admin/statement</t>
+  </si>
+  <si>
+    <t>http://localhost:8085/document/{statementId}</t>
+  </si>
+  <si>
+    <t>http://localhost:8085/document/{statementId}/sign</t>
+  </si>
+  <si>
+    <t>http://localhost:8085/document/{statementId}/sign/code</t>
   </si>
 </sst>
 </file>
@@ -198,16 +222,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -492,7 +516,7 @@
   <dimension ref="A1:AF24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z3" sqref="Z3:Z5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,20 +664,20 @@
       <c r="A3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="7">
         <v>400</v>
       </c>
-      <c r="D3" s="5"/>
+      <c r="D3" s="7"/>
       <c r="H3">
         <v>500</v>
       </c>
       <c r="I3" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="K3" s="4">
@@ -668,7 +692,7 @@
       <c r="Q3" t="s">
         <v>32</v>
       </c>
-      <c r="R3" s="8" t="s">
+      <c r="R3" s="5" t="s">
         <v>37</v>
       </c>
       <c r="T3">
@@ -680,7 +704,7 @@
       <c r="Y3" t="s">
         <v>20</v>
       </c>
-      <c r="Z3" s="8" t="s">
+      <c r="Z3" s="5" t="s">
         <v>35</v>
       </c>
     </row>
@@ -688,7 +712,7 @@
       <c r="A4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="5" t="s">
         <v>40</v>
       </c>
       <c r="C4" s="3"/>
@@ -702,7 +726,7 @@
       <c r="I4" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="M4" s="4">
@@ -714,7 +738,7 @@
       <c r="Q4" t="s">
         <v>22</v>
       </c>
-      <c r="R4" s="8" t="s">
+      <c r="R4" s="5" t="s">
         <v>38</v>
       </c>
       <c r="U4">
@@ -728,7 +752,9 @@
       <c r="A5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
       <c r="E5">
         <v>404</v>
       </c>
@@ -742,7 +768,7 @@
       <c r="Q5" t="s">
         <v>23</v>
       </c>
-      <c r="R5" s="8" t="s">
+      <c r="R5" s="5" t="s">
         <v>2</v>
       </c>
       <c r="U5">
@@ -757,7 +783,7 @@
       <c r="Y5" t="s">
         <v>23</v>
       </c>
-      <c r="Z5" s="8" t="s">
+      <c r="Z5" s="5" t="s">
         <v>36</v>
       </c>
       <c r="AD5">
@@ -768,7 +794,9 @@
       <c r="A6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
       <c r="E6">
         <v>404</v>
       </c>
@@ -779,7 +807,7 @@
       <c r="Q6" t="s">
         <v>25</v>
       </c>
-      <c r="R6" s="8" t="s">
+      <c r="R6" s="5" t="s">
         <v>3</v>
       </c>
       <c r="U6">
@@ -793,7 +821,9 @@
       <c r="A7" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="E7">
         <v>404</v>
       </c>
@@ -804,7 +834,7 @@
       <c r="Q7" t="s">
         <v>33</v>
       </c>
-      <c r="R7" s="8" t="s">
+      <c r="R7" s="5" t="s">
         <v>4</v>
       </c>
       <c r="U7">
@@ -818,7 +848,9 @@
       <c r="A8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="E8">
         <v>404</v>
       </c>
@@ -829,7 +861,7 @@
       <c r="Q8" t="s">
         <v>27</v>
       </c>
-      <c r="R8" s="8" t="s">
+      <c r="R8" s="5" t="s">
         <v>5</v>
       </c>
       <c r="U8">
@@ -843,7 +875,9 @@
       <c r="A9" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="E9">
         <v>404</v>
       </c>
@@ -857,7 +891,7 @@
       <c r="Q9" t="s">
         <v>28</v>
       </c>
-      <c r="R9" s="8" t="s">
+      <c r="R9" s="5" t="s">
         <v>6</v>
       </c>
       <c r="U9">
@@ -874,7 +908,9 @@
       <c r="A10" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
       <c r="E10">
         <v>404</v>
       </c>
@@ -882,7 +918,7 @@
       <c r="Q10" t="s">
         <v>29</v>
       </c>
-      <c r="R10" s="8" t="s">
+      <c r="R10" s="5" t="s">
         <v>7</v>
       </c>
       <c r="U10">
@@ -893,7 +929,9 @@
       <c r="A11" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="1"/>
+      <c r="B11" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="E11">
         <v>404</v>
       </c>
@@ -901,7 +939,7 @@
       <c r="Q11" t="s">
         <v>30</v>
       </c>
-      <c r="R11" s="8" t="s">
+      <c r="R11" s="5" t="s">
         <v>8</v>
       </c>
       <c r="U11">
@@ -912,12 +950,14 @@
       <c r="A12" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="J12" s="1"/>
       <c r="Q12" t="s">
         <v>31</v>
       </c>
-      <c r="R12" s="8" t="s">
+      <c r="R12" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -990,37 +1030,37 @@
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="7"/>
+      <c r="B3" s="8"/>
       <c r="C3">
         <v>404</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="7"/>
+      <c r="B4" s="8"/>
       <c r="C4">
         <v>406</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="7"/>
+      <c r="B5" s="8"/>
       <c r="C5">
         <v>406</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="7"/>
+      <c r="B6" s="8"/>
       <c r="C6">
         <v>500</v>
       </c>

</xml_diff>

<commit_message>
feature: add pagination for all statements in MS deal and MS gateway
</commit_message>
<xml_diff>
--- a/methods.xlsx
+++ b/methods.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20384"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42252187-3D2F-434A-8E9F-666992F34CF2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBC97FC-EE82-4DD8-9A47-338FA579685A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Методы" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="50">
   <si>
     <t>http://localhost:8083/statement</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>http://localhost:8085/document/{statementId}/sign/code</t>
+  </si>
+  <si>
+    <t>InvalidPreApproveException</t>
   </si>
 </sst>
 </file>
@@ -513,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF24"/>
+  <dimension ref="A1:AJ24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,25 +529,30 @@
     <col min="3" max="4" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="61.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="24" width="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="36" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="30" width="4" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.7109375" customWidth="1"/>
+    <col min="18" max="18" width="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="61.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="25" width="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4" customWidth="1"/>
+    <col min="27" max="27" width="4" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="36" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="33" width="4" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="3.7109375" customWidth="1"/>
+    <col min="36" max="36" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>10</v>
       </c>
@@ -555,38 +563,42 @@
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="6"/>
+      <c r="J1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="6"/>
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
       <c r="T1" s="6"/>
       <c r="U1" s="6"/>
       <c r="V1" s="6"/>
       <c r="W1" s="6"/>
       <c r="X1" s="6"/>
-      <c r="Y1" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="Y1" s="6"/>
       <c r="Z1" s="6"/>
       <c r="AA1" s="6"/>
-      <c r="AB1" s="6"/>
+      <c r="AB1" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="AC1" s="6"/>
       <c r="AD1" s="6"/>
       <c r="AE1" s="6"/>
       <c r="AF1" s="6"/>
-    </row>
-    <row r="2" spans="1:32" ht="181.5" x14ac:dyDescent="0.25">
+      <c r="AG1" s="6"/>
+      <c r="AH1" s="6"/>
+      <c r="AI1" s="6"/>
+      <c r="AJ1" s="6"/>
+    </row>
+    <row r="2" spans="1:36" ht="181.5" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
@@ -603,64 +615,76 @@
         <v>14</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AG2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AH2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AI2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -671,44 +695,44 @@
         <v>400</v>
       </c>
       <c r="D3" s="7"/>
-      <c r="H3">
-        <v>500</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="I3">
+        <v>500</v>
+      </c>
+      <c r="J3" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>0</v>
-      </c>
-      <c r="K3" s="4">
-        <v>400</v>
       </c>
       <c r="L3" s="4">
         <v>400</v>
       </c>
-      <c r="P3">
-        <v>500</v>
-      </c>
-      <c r="Q3" t="s">
+      <c r="M3" s="4">
+        <v>400</v>
+      </c>
+      <c r="R3">
+        <v>500</v>
+      </c>
+      <c r="S3" t="s">
         <v>32</v>
       </c>
-      <c r="R3" s="5" t="s">
+      <c r="T3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="T3">
+      <c r="V3">
         <v>400</v>
       </c>
-      <c r="X3">
-        <v>500</v>
-      </c>
-      <c r="Y3" t="s">
+      <c r="AA3">
+        <v>500</v>
+      </c>
+      <c r="AB3" t="s">
         <v>20</v>
       </c>
-      <c r="Z3" s="5" t="s">
+      <c r="AC3" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -720,35 +744,35 @@
       <c r="E4">
         <v>404</v>
       </c>
-      <c r="H4">
-        <v>500</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="I4">
+        <v>500</v>
+      </c>
+      <c r="J4" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="M4" s="4">
-        <v>404</v>
-      </c>
-      <c r="P4">
-        <v>500</v>
-      </c>
-      <c r="Q4" t="s">
+      <c r="N4" s="4">
+        <v>404</v>
+      </c>
+      <c r="R4">
+        <v>500</v>
+      </c>
+      <c r="S4" t="s">
         <v>22</v>
       </c>
-      <c r="R4" s="5" t="s">
+      <c r="T4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="U4">
-        <v>404</v>
-      </c>
-      <c r="X4">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="W4">
+        <v>404</v>
+      </c>
+      <c r="AA4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -762,35 +786,41 @@
         <v>406</v>
       </c>
       <c r="H5">
-        <v>500</v>
-      </c>
-      <c r="J5" s="1"/>
-      <c r="Q5" t="s">
+        <v>428</v>
+      </c>
+      <c r="I5">
+        <v>500</v>
+      </c>
+      <c r="K5" s="1"/>
+      <c r="S5" t="s">
         <v>23</v>
       </c>
-      <c r="R5" s="5" t="s">
+      <c r="T5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="U5">
-        <v>404</v>
-      </c>
-      <c r="V5">
+      <c r="W5">
+        <v>404</v>
+      </c>
+      <c r="X5">
         <v>406</v>
       </c>
-      <c r="X5">
-        <v>500</v>
-      </c>
-      <c r="Y5" t="s">
+      <c r="Z5">
+        <v>428</v>
+      </c>
+      <c r="AA5">
+        <v>500</v>
+      </c>
+      <c r="AB5" t="s">
         <v>23</v>
       </c>
-      <c r="Z5" s="5" t="s">
+      <c r="AC5" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AD5">
+      <c r="AG5">
         <v>406</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -800,24 +830,24 @@
       <c r="E6">
         <v>404</v>
       </c>
-      <c r="H6">
-        <v>500</v>
-      </c>
-      <c r="J6" s="1"/>
-      <c r="Q6" t="s">
+      <c r="I6">
+        <v>500</v>
+      </c>
+      <c r="K6" s="1"/>
+      <c r="S6" t="s">
         <v>25</v>
       </c>
-      <c r="R6" s="5" t="s">
+      <c r="T6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="U6">
-        <v>404</v>
-      </c>
-      <c r="X6">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="W6">
+        <v>404</v>
+      </c>
+      <c r="AA6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -827,24 +857,24 @@
       <c r="E7">
         <v>404</v>
       </c>
-      <c r="H7">
-        <v>500</v>
-      </c>
-      <c r="J7" s="1"/>
-      <c r="Q7" t="s">
+      <c r="I7">
+        <v>500</v>
+      </c>
+      <c r="K7" s="1"/>
+      <c r="S7" t="s">
         <v>33</v>
       </c>
-      <c r="R7" s="5" t="s">
+      <c r="T7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="U7">
-        <v>404</v>
-      </c>
-      <c r="X7">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="W7">
+        <v>404</v>
+      </c>
+      <c r="AA7">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -854,24 +884,24 @@
       <c r="E8">
         <v>404</v>
       </c>
-      <c r="H8">
-        <v>500</v>
-      </c>
-      <c r="J8" s="1"/>
-      <c r="Q8" t="s">
+      <c r="I8">
+        <v>500</v>
+      </c>
+      <c r="K8" s="1"/>
+      <c r="S8" t="s">
         <v>27</v>
       </c>
-      <c r="R8" s="5" t="s">
+      <c r="T8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="U8">
-        <v>404</v>
-      </c>
-      <c r="X8">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="W8">
+        <v>404</v>
+      </c>
+      <c r="AA8">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -884,27 +914,27 @@
       <c r="G9">
         <v>406</v>
       </c>
-      <c r="H9">
-        <v>500</v>
-      </c>
-      <c r="J9" s="1"/>
-      <c r="Q9" t="s">
+      <c r="I9">
+        <v>500</v>
+      </c>
+      <c r="K9" s="1"/>
+      <c r="S9" t="s">
         <v>28</v>
       </c>
-      <c r="R9" s="5" t="s">
+      <c r="T9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="U9">
-        <v>404</v>
-      </c>
       <c r="W9">
+        <v>404</v>
+      </c>
+      <c r="Y9">
         <v>406</v>
       </c>
-      <c r="X9">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AA9">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -914,18 +944,18 @@
       <c r="E10">
         <v>404</v>
       </c>
-      <c r="J10" s="1"/>
-      <c r="Q10" t="s">
+      <c r="K10" s="1"/>
+      <c r="S10" t="s">
         <v>29</v>
       </c>
-      <c r="R10" s="5" t="s">
+      <c r="T10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="U10">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="W10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -935,29 +965,29 @@
       <c r="E11">
         <v>404</v>
       </c>
-      <c r="J11" s="1"/>
-      <c r="Q11" t="s">
+      <c r="K11" s="1"/>
+      <c r="S11" t="s">
         <v>30</v>
       </c>
-      <c r="R11" s="5" t="s">
+      <c r="T11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="U11">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="W11">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>31</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J12" s="1"/>
-      <c r="Q12" t="s">
+      <c r="K12" s="1"/>
+      <c r="S12" t="s">
         <v>31</v>
       </c>
-      <c r="R12" s="5" t="s">
+      <c r="T12" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -981,10 +1011,10 @@
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="I1:P1"/>
-    <mergeCell ref="Q1:X1"/>
-    <mergeCell ref="Y1:AF1"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="J1:R1"/>
+    <mergeCell ref="S1:AA1"/>
+    <mergeCell ref="AB1:AJ1"/>
     <mergeCell ref="C3:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -993,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E15712-D58D-4025-B723-5D6A6C349C09}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1058,20 +1088,30 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7">
         <v>500</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>